<commit_message>
Se modifica la generación del nemotecnico para la compra de Simultaneas
Además se modifico la fecha de pago para que sea igual a la fecha de ingreso. Se aprovecha de generar el reporte para el 20241125.
</commit_message>
<xml_diff>
--- a/Nevasa/InformeCompleto/20241125/20241125_informe_completo_results.xlsx
+++ b/Nevasa/InformeCompleto/20241125/20241125_informe_completo_results.xlsx
@@ -496,7 +496,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>45677</v>
+        <v>45621</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>45621</v>
@@ -515,7 +515,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>BCI</t>
+          <t>SMT_20012025_25112024_0.52_BCI</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -536,7 +536,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>45649</v>
+        <v>45621</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>45621</v>
@@ -555,7 +555,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>ORO BLANCO</t>
+          <t>SMT_23122024_25112024_0.56_ORO_BLANCO</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -576,7 +576,7 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>45649</v>
+        <v>45621</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>45621</v>
@@ -595,7 +595,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>ORO BLANCO</t>
+          <t>SMT_23122024_25112024_0.56_ORO_BLANCO</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">

</xml_diff>